<commit_message>
Parsing of positive and negative expressions added
</commit_message>
<xml_diff>
--- a/MathChamp - Test Plan.xlsx
+++ b/MathChamp - Test Plan.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30e40e6088cd9960/Documents/My Documents/1. University Documents/2. Advanced Programming Concepts and Techniques/Code/MathChamp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30e40e6088cd9960/Documents/My Documents/1. University Documents/2. Advanced Programming Concepts and Techniques/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="8_{66D637F1-F5DD-43E0-BC34-F3155DA2AAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83089BFA-2BF5-45D1-8761-A00E914492B7}"/>
+  <xr:revisionPtr revIDLastSave="539" documentId="8_{66D637F1-F5DD-43E0-BC34-F3155DA2AAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{157112DA-E13E-48FC-BAD3-D62FC2E8F5EE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2550DACF-A7A3-480B-86AF-FC498795188B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2550DACF-A7A3-480B-86AF-FC498795188B}"/>
   </bookViews>
   <sheets>
     <sheet name="MathChamp Interpreter - Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="MathChamp - Identified Issues" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="153">
   <si>
     <t>MathChamp Interpreter: Test Plan</t>
   </si>
@@ -56,9 +57,6 @@
     <t>EXEPECTED OUTPUT</t>
   </si>
   <si>
-    <t>ACTUAL RESULT</t>
-  </si>
-  <si>
     <t>COMMENTS</t>
   </si>
   <si>
@@ -215,54 +213,18 @@
     <t>3 * 4</t>
   </si>
   <si>
-    <t>INTEGER(1,2) and PLUS+ were displayed</t>
-  </si>
-  <si>
     <t>1 - 3</t>
   </si>
   <si>
-    <t>INTEGER(1,3) and MINUS- were displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(3,4) and MULTIPLY* were displayed</t>
-  </si>
-  <si>
     <t>5 * 6</t>
   </si>
   <si>
-    <t>INTEGER(1,3) and MINUS- displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(1,2) and PLUS+ displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(3,4) and MULTIPLY* displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(5,6) and MULTIPILY* displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(5+,6) and MULTIPLY* were displayed</t>
-  </si>
-  <si>
     <t>7 - 8</t>
   </si>
   <si>
-    <t>INTEGER(7,8) and MINUS* displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(7,8) and MINUS* were displayed</t>
-  </si>
-  <si>
     <t>9 + 10</t>
   </si>
   <si>
-    <t>INTEGER(9,10) and PLUS+ displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(9,10) and PLUS+ were displayed</t>
-  </si>
-  <si>
     <t>Enter 12345 + 678910, return</t>
   </si>
   <si>
@@ -287,9 +249,6 @@
     <t>12345 + 678910</t>
   </si>
   <si>
-    <t>INTEGER(1,2,3,4,5,6,7,8,9,10) and PLUS+ displayed</t>
-  </si>
-  <si>
     <t>Enter 10 + (2*3), return</t>
   </si>
   <si>
@@ -299,26 +258,265 @@
     <t>Enter 12 + (5*3), return</t>
   </si>
   <si>
-    <t>INTEGER(10,2,3) and each ( ) and * displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(10,2,3) and each ( ) and * were displayed</t>
-  </si>
-  <si>
     <t>12 + (5*3.2)</t>
   </si>
   <si>
-    <t>INTEGER(12,5,3,2) and each ( ) and * FLOAT. displayed</t>
-  </si>
-  <si>
-    <t>INTEGER(12,5,3,2) and each ( ) and * FLOAT. were displayed</t>
+    <t>Tokens are allocated to expression (minus ints)</t>
+  </si>
+  <si>
+    <t>-1 + -2</t>
+  </si>
+  <si>
+    <t>-3 + -4</t>
+  </si>
+  <si>
+    <t>-5 + -6</t>
+  </si>
+  <si>
+    <t>Enter -3 + -4, return</t>
+  </si>
+  <si>
+    <t>Enter -1 + -2, return</t>
+  </si>
+  <si>
+    <t>Enter -5 + -6, return</t>
+  </si>
+  <si>
+    <t>Enter -7 * -8, return</t>
+  </si>
+  <si>
+    <t>-7 * -8</t>
+  </si>
+  <si>
+    <t>Enter -9 - -10, return</t>
+  </si>
+  <si>
+    <t>-9 - -10</t>
+  </si>
+  <si>
+    <t>Enter 12 / -2, return</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12 / -2</t>
+  </si>
+  <si>
+    <t>14 - (-2 * 3)</t>
+  </si>
+  <si>
+    <t>Successful parse and calculation of input</t>
+  </si>
+  <si>
+    <t>INTEGER(1,2) and PLUS+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEGER(1,3) and MINUS- </t>
+  </si>
+  <si>
+    <t>INTEGER(3,4) and MULTIPLY*</t>
+  </si>
+  <si>
+    <t>INTEGER(5,6) and MULTIPILY*</t>
+  </si>
+  <si>
+    <t>INTEGER(9,10) and PLUS+</t>
+  </si>
+  <si>
+    <t>INTEGER(7,8) and MINUS*</t>
+  </si>
+  <si>
+    <t>INTEGER(1,2,3,4,5,6,7,8,9,10) and PLUS+</t>
+  </si>
+  <si>
+    <t>INTEGER(12,5,3,2) and each ( ) and * FLOAT.</t>
+  </si>
+  <si>
+    <t>INTEGER(10,2,3) and each ( ) and *</t>
+  </si>
+  <si>
+    <t>INTEGER(-1,-2) and PLUS+</t>
+  </si>
+  <si>
+    <t>INTEGER(-3,-4) and PLUS+</t>
+  </si>
+  <si>
+    <t>INTEGER(-5,-6) and PLUS+</t>
+  </si>
+  <si>
+    <t>INTEGER(-7,-8) and MULTIPLY*</t>
+  </si>
+  <si>
+    <t>INTEGER(-9,-10) and MINUS-</t>
+  </si>
+  <si>
+    <t>INTEGER(12,-2) and DIVIDE/</t>
+  </si>
+  <si>
+    <t>INTEGER(14,-2,3) and each ( ) and MINUS- and MULTIPLY*</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+  </si>
+  <si>
+    <t>INTEGER(1,3) and MINUS-</t>
+  </si>
+  <si>
+    <t>INTEGER(5+,6) and MULTIPLY*</t>
+  </si>
+  <si>
+    <t>INTEGER(10,2,3) and each ( ) and MULTIPLY*</t>
+  </si>
+  <si>
+    <t>Enter 1 + 2 + 3 + 4 + 5, return</t>
+  </si>
+  <si>
+    <t>1 + 2 + 3 + 4 + 5</t>
+  </si>
+  <si>
+    <t>1 * 10 * 100</t>
+  </si>
+  <si>
+    <t>Enter 14 - (-2 * 3), return</t>
+  </si>
+  <si>
+    <t>Enter 1 * 10 * 100, return</t>
+  </si>
+  <si>
+    <t>1 - 5 - 10</t>
+  </si>
+  <si>
+    <t>Enter 1 - 5 - 10, return</t>
+  </si>
+  <si>
+    <t>Enter 20 / 100 / 10, return</t>
+  </si>
+  <si>
+    <t>-0.02</t>
+  </si>
+  <si>
+    <t>Enter 500 + 2 * 5 / 4 - 8, return</t>
+  </si>
+  <si>
+    <t>Enter 950 / (5*2) - 10, return</t>
+  </si>
+  <si>
+    <t>950 / (5*2) - 10</t>
+  </si>
+  <si>
+    <t>(90 + 10) + (10 * 2) * (6 - 5) - (4 / 2)</t>
+  </si>
+  <si>
+    <t>10 + (5+2) * (5*3) - (9-2) / (1/2)</t>
+  </si>
+  <si>
+    <t>500 + 2 * 5 / 4 - 8</t>
+  </si>
+  <si>
+    <t>line 37, in get_next_token, self.parenthesis_count += 1, AttributeError: 'Parser' object has no attribute 'parenthesis_count'</t>
+  </si>
+  <si>
+    <t>COMMENTS/ERROR(S)</t>
+  </si>
+  <si>
+    <t>CRASHED PROGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 * (5 / 2)</t>
+  </si>
+  <si>
+    <t>(5 / 2) * 10</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">line 37, in get_next_token, self.parenthesis_count += 1, AttributeError: 'Parser' object has no attribute 'parenthesis_count' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAUSED BY STARTING WITH PARANTHESIS</t>
+    </r>
+  </si>
+  <si>
+    <t>Successful parse and calculation of negative number input</t>
+  </si>
+  <si>
+    <t>Enter 10 + (5+2) * (5*3) - (9-2) / (1/2), return</t>
+  </si>
+  <si>
+    <t>Enter (90 + 10) + (10 * 2) * (6 - 5) - (4 / 2), return</t>
+  </si>
+  <si>
+    <t>Enter (5 / 2) * 10, return</t>
+  </si>
+  <si>
+    <t>Enter 10 * (5 / 2), return</t>
+  </si>
+  <si>
+    <t>ERROR ID</t>
+  </si>
+  <si>
+    <t>er1</t>
+  </si>
+  <si>
+    <t>er2</t>
+  </si>
+  <si>
+    <t>MathChamp Interpreter: Identified Issues</t>
+  </si>
+  <si>
+    <t>ERROR DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ISSUE</t>
+  </si>
+  <si>
+    <t>PROGRAM CRASH - "Invalid Expression"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line 37, in get_next_token, self.parenthesis_count += 1, AttributeError: 'Parser' object has no attribute 'parenthesis_count' </t>
+  </si>
+  <si>
+    <t>CAUSED BY STARTING WITH PARANTHESIS</t>
+  </si>
+  <si>
+    <t>2 + -1</t>
+  </si>
+  <si>
+    <t>Enter 2 + -1, return</t>
+  </si>
+  <si>
+    <t>Enter 20 * -2, return</t>
+  </si>
+  <si>
+    <t>20 * -2</t>
+  </si>
+  <si>
+    <t>Enter 40 / -10, return</t>
+  </si>
+  <si>
+    <t>40 / -10</t>
+  </si>
+  <si>
+    <t>40 + 6 / (4 - 5) - -10</t>
+  </si>
+  <si>
+    <t>Enter 40 + 6 / (4 - 5) - -10, return</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,14 +554,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="9"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,16 +561,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="9"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -403,11 +639,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,36 +667,208 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
-        <i/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -457,10 +878,14 @@
       <font>
         <i/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -471,14 +896,36 @@
     </dxf>
     <dxf>
       <font>
-        <i/>
+        <i val="0"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -494,7 +941,9 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -521,10 +970,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -592,6 +1038,9 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -622,19 +1071,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E450872-46DF-4A3C-BD66-0891C0DB87E4}" name="Table1" displayName="Table1" ref="A3:H50" totalsRowShown="0" headerRowDxfId="9" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E450872-46DF-4A3C-BD66-0891C0DB87E4}" name="Table1" displayName="Table1" ref="A3:H50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A3:H50" xr:uid="{2E450872-46DF-4A3C-BD66-0891C0DB87E4}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2A1C62DC-7615-47AA-BE31-3F6BBA36C62E}" name="TEST NO" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{986996CD-5EE4-4522-B08F-E76D83A83D4C}" name="TEST ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{FE730A53-5EEF-4A76-BCD9-2A805E39482D}" name="OBJECTIVE" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{4B96D5CC-2EAF-4A43-8704-8ABDE2CD6F46}" name="STEPS" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{94AF5410-28EC-43D6-BB8D-0CA5EEAE7B73}" name="INPUT" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{1EA1E4D4-1533-438A-BF78-61C21075C0C6}" name="EXEPECTED OUTPUT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F106BA7F-BA18-414A-82D0-4EF16551729D}" name="ACTUAL RESULT" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{BE678DB3-711B-4929-81C6-B84C97563F39}" name="COMMENTS" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2A1C62DC-7615-47AA-BE31-3F6BBA36C62E}" name="TEST NO" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{986996CD-5EE4-4522-B08F-E76D83A83D4C}" name="TEST ID" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{FE730A53-5EEF-4A76-BCD9-2A805E39482D}" name="OBJECTIVE" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{4B96D5CC-2EAF-4A43-8704-8ABDE2CD6F46}" name="STEPS" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{94AF5410-28EC-43D6-BB8D-0CA5EEAE7B73}" name="INPUT" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{1EA1E4D4-1533-438A-BF78-61C21075C0C6}" name="EXEPECTED OUTPUT" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{F106BA7F-BA18-414A-82D0-4EF16551729D}" name="OUTPUT" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{BE678DB3-711B-4929-81C6-B84C97563F39}" name="COMMENTS/ERROR(S)" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51536A3D-D140-4760-98C2-8F29F192E818}" name="Table2" displayName="Table2" ref="A4:E25" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="6">
+  <autoFilter ref="A4:E25" xr:uid="{51536A3D-D140-4760-98C2-8F29F192E818}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0215BD31-DDF8-4299-B6FC-FFE5C32C38CD}" name="Error" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{4C3E167D-F091-46DB-9E55-A98E586F6F59}" name="ERROR ID" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{4330AAF2-23C8-4315-BE23-84C064621338}" name="ISSUE" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A235DADF-B4F0-43EF-A6D6-64A4C188D5A7}" name="ERROR DESCRIPTION" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{6AE35E81-F80B-47F9-8503-50D2DD844005}" name="COMMENTS" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -906,36 +1369,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14B6601-0E27-48C2-8B67-D3F95DE45290}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.8984375" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="32.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.796875" customWidth="1"/>
-    <col min="5" max="5" width="19.296875" customWidth="1"/>
-    <col min="6" max="6" width="48.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.09765625" customWidth="1"/>
+    <col min="3" max="3" width="55.5" customWidth="1"/>
+    <col min="4" max="4" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="55.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -950,766 +1412,1194 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>65</v>
+      <c r="F4" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>83</v>
+        <v>62</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>87</v>
+        <v>70</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>90</v>
+        <v>72</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="7">
+        <v>15</v>
+      </c>
+      <c r="G20" s="8">
+        <v>15</v>
+      </c>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1000</v>
+      </c>
+      <c r="G21" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="7">
+        <v>-14</v>
+      </c>
+      <c r="G22" s="8">
+        <v>-14</v>
+      </c>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="7">
+        <v>494.5</v>
+      </c>
+      <c r="G24" s="8">
+        <v>494.5</v>
+      </c>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="7">
+        <v>85</v>
+      </c>
+      <c r="G25" s="8">
+        <v>85</v>
+      </c>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="7">
+        <v>101</v>
+      </c>
+      <c r="G26" s="8">
+        <v>101</v>
+      </c>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="7">
+        <v>118</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="7">
+        <v>25</v>
+      </c>
+      <c r="G28" s="8">
+        <v>25</v>
+      </c>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="7">
+        <v>25</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8">
+        <v>1</v>
+      </c>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F31" s="7">
+        <v>-40</v>
+      </c>
+      <c r="G31" s="8">
+        <v>-40</v>
+      </c>
+      <c r="H31" s="11"/>
+    </row>
+    <row r="32" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="7">
+        <v>-4</v>
+      </c>
+      <c r="G32" s="8">
+        <v>-4</v>
+      </c>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>30</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="7">
+        <v>44</v>
+      </c>
+      <c r="G33" s="8">
+        <v>44</v>
+      </c>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>32</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="8"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="8"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="11"/>
+    </row>
+    <row r="37" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="8"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="8"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>36</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="8"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="8"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="8"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="42" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>39</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="8"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="7"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>40</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="8"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="7"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="8"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="7"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>42</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="8"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="7"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="9"/>
-    </row>
-    <row r="46" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="8"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>44</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="8"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="7"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="7"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="9"/>
-    </row>
-    <row r="49" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>46</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="8"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="7"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="9"/>
-    </row>
-    <row r="50" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="11"/>
+    </row>
+    <row r="50" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>47</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="8"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="7"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="9"/>
+      <c r="H50" s="11"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E23" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3F10F0-99DA-4AAD-92A9-79519DDF818A}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
+    <col min="3" max="3" width="37.59765625" customWidth="1"/>
+    <col min="4" max="4" width="89.19921875" customWidth="1"/>
+    <col min="5" max="5" width="37.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modulo and variable assignment, updated errors
</commit_message>
<xml_diff>
--- a/MathChamp - Test Plan.xlsx
+++ b/MathChamp - Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30e40e6088cd9960/Documents/My Documents/1. University Documents/2. Advanced Programming Concepts and Techniques/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="539" documentId="8_{66D637F1-F5DD-43E0-BC34-F3155DA2AAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{157112DA-E13E-48FC-BAD3-D62FC2E8F5EE}"/>
+  <xr:revisionPtr revIDLastSave="739" documentId="8_{66D637F1-F5DD-43E0-BC34-F3155DA2AAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{499E330B-C7B1-4468-9A24-403D7CB54AB8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2550DACF-A7A3-480B-86AF-FC498795188B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2550DACF-A7A3-480B-86AF-FC498795188B}"/>
   </bookViews>
   <sheets>
     <sheet name="MathChamp Interpreter - Testing" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="262">
   <si>
     <t>MathChamp Interpreter: Test Plan</t>
   </si>
@@ -510,6 +510,333 @@
   </si>
   <si>
     <t>Enter 40 + 6 / (4 - 5) - -10, return</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>RESOLVED</t>
+  </si>
+  <si>
+    <t>2 ^ 4</t>
+  </si>
+  <si>
+    <t>Enter 2 + 3 ^ 4, return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 + 3 ^ 4 </t>
+  </si>
+  <si>
+    <t>Enter 2 ^ 4, return</t>
+  </si>
+  <si>
+    <t>Enter 2 * 1 + 3 ^ 3, return</t>
+  </si>
+  <si>
+    <t>2 * 1 + 3 ^ 3</t>
+  </si>
+  <si>
+    <t>Enter 6 / 2 + 4 ^ 6, return</t>
+  </si>
+  <si>
+    <t>6 / 2 + 4 ^ 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 ^ 2 - 4 </t>
+  </si>
+  <si>
+    <t>Enter 8 ^ 2 -4, return</t>
+  </si>
+  <si>
+    <t>CALULATION ISSUE - Power To</t>
+  </si>
+  <si>
+    <t>Multiplication has higher prcedence than power-to, causing incorrect calculation</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Enter 3 - 4 + 9^2 * (10 * 2), return</t>
+  </si>
+  <si>
+    <t>3 - 4 + 9^2 * (10 * 2)</t>
+  </si>
+  <si>
+    <t>Enter 14 * 2 + 9 - 4 / 1 ^ 3, return</t>
+  </si>
+  <si>
+    <t>14 * 2 + 9 - 4 / 1 ^3</t>
+  </si>
+  <si>
+    <t>Calculation error due to precedence of multiplication</t>
+  </si>
+  <si>
+    <t>Enter 14 * 2 + 9 - 4 /(1 ^3), return</t>
+  </si>
+  <si>
+    <t>14 * 2 + 9 - 4 /(1 ^3)</t>
+  </si>
+  <si>
+    <t>Correct output by placing power-to in paranthesis, evidencing precedence issue</t>
+  </si>
+  <si>
+    <t>Variable assignment</t>
+  </si>
+  <si>
+    <t>Enter x = 2, return</t>
+  </si>
+  <si>
+    <t>x = 2</t>
+  </si>
+  <si>
+    <t>Enter x = 2, return, enter x + 4</t>
+  </si>
+  <si>
+    <t>x = 2, x + 4</t>
+  </si>
+  <si>
+    <t>Enter x = 4 *2, return</t>
+  </si>
+  <si>
+    <t>x = 4 *2</t>
+  </si>
+  <si>
+    <t>Enter x = 10, return, enter x / 2</t>
+  </si>
+  <si>
+    <t>x = 10, x / 2</t>
+  </si>
+  <si>
+    <t>Enter x = 140, return, enter x - 100</t>
+  </si>
+  <si>
+    <t>Enter x = 1000, return, enter x %16</t>
+  </si>
+  <si>
+    <t>x = 140, x - 100</t>
+  </si>
+  <si>
+    <t>x = 1000, x % 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter x = 10, return, enter y = 30, return, enter x + y </t>
+  </si>
+  <si>
+    <t>x = 10, y = 30, x + y</t>
+  </si>
+  <si>
+    <t>Enter x = 100, return, enter y = 2, return, enter x / y</t>
+  </si>
+  <si>
+    <t>x = 100, y = 2, x / y</t>
+  </si>
+  <si>
+    <t>x = 1000, y = 6, x % y</t>
+  </si>
+  <si>
+    <t>Enter x = 10000, return, enter y = 6, return, enter x % y</t>
+  </si>
+  <si>
+    <t>tc48</t>
+  </si>
+  <si>
+    <t>tc49</t>
+  </si>
+  <si>
+    <t>tc50</t>
+  </si>
+  <si>
+    <t>tc51</t>
+  </si>
+  <si>
+    <t>tc52</t>
+  </si>
+  <si>
+    <t>tc53</t>
+  </si>
+  <si>
+    <t>tc54</t>
+  </si>
+  <si>
+    <t>Enter x = 200 =, return, y = 400, y - x</t>
+  </si>
+  <si>
+    <t>x = 200, y = 400, y - x</t>
+  </si>
+  <si>
+    <t>Enter x = 500, x / (1 + 2)</t>
+  </si>
+  <si>
+    <t>x = 500, x / (1 + 2)</t>
+  </si>
+  <si>
+    <t>Successful parse and calculation of modulo %</t>
+  </si>
+  <si>
+    <t>Successful parse and calculation of power-to input ^</t>
+  </si>
+  <si>
+    <t>Enter 100 % 7.5</t>
+  </si>
+  <si>
+    <t>100 % 7.5</t>
+  </si>
+  <si>
+    <t>Enter 500 % 42 + 5</t>
+  </si>
+  <si>
+    <t>500 % 42 + 5</t>
+  </si>
+  <si>
+    <t>4000 % 67 * 2</t>
+  </si>
+  <si>
+    <t>Enter 4000 % 67 * 2</t>
+  </si>
+  <si>
+    <t>59 % 5 - (3  + 4)</t>
+  </si>
+  <si>
+    <t>Enter 59 % 5 - (3  + 4)</t>
+  </si>
+  <si>
+    <t>6004.25 % 46 / ( 16 - 2)</t>
+  </si>
+  <si>
+    <t>Enter 6004.25 % 46 / ( 16 - 2)</t>
+  </si>
+  <si>
+    <t>tc55</t>
+  </si>
+  <si>
+    <t>tc56</t>
+  </si>
+  <si>
+    <t>tc57</t>
+  </si>
+  <si>
+    <t>tc58</t>
+  </si>
+  <si>
+    <t>tc59</t>
+  </si>
+  <si>
+    <t>tc60</t>
+  </si>
+  <si>
+    <t>tc61</t>
+  </si>
+  <si>
+    <t>tc62</t>
+  </si>
+  <si>
+    <t>tc63</t>
+  </si>
+  <si>
+    <t>tc64</t>
+  </si>
+  <si>
+    <t>tc65</t>
+  </si>
+  <si>
+    <t>tc66</t>
+  </si>
+  <si>
+    <t>tc67</t>
+  </si>
+  <si>
+    <t>tc68</t>
+  </si>
+  <si>
+    <t>tc69</t>
+  </si>
+  <si>
+    <t>tc70</t>
+  </si>
+  <si>
+    <t>tc71</t>
+  </si>
+  <si>
+    <t>tc72</t>
+  </si>
+  <si>
+    <t>tc73</t>
+  </si>
+  <si>
+    <t>tc74</t>
+  </si>
+  <si>
+    <t>tc75</t>
+  </si>
+  <si>
+    <t>tc76</t>
+  </si>
+  <si>
+    <t>tc77</t>
+  </si>
+  <si>
+    <t>tc78</t>
+  </si>
+  <si>
+    <t>tc79</t>
+  </si>
+  <si>
+    <t>tc80</t>
+  </si>
+  <si>
+    <t>tc81</t>
+  </si>
+  <si>
+    <t>tc82</t>
+  </si>
+  <si>
+    <t>tc83</t>
+  </si>
+  <si>
+    <t>tc84</t>
+  </si>
+  <si>
+    <t>tc85</t>
+  </si>
+  <si>
+    <t>tc86</t>
+  </si>
+  <si>
+    <t>tc87</t>
+  </si>
+  <si>
+    <t>tc88</t>
+  </si>
+  <si>
+    <t>tc89</t>
+  </si>
+  <si>
+    <t>tc90</t>
+  </si>
+  <si>
+    <t>tc91</t>
+  </si>
+  <si>
+    <t>tc92</t>
+  </si>
+  <si>
+    <t>tc93</t>
+  </si>
+  <si>
+    <t>tc94</t>
+  </si>
+  <si>
+    <t>tc95</t>
+  </si>
+  <si>
+    <t>tc96</t>
+  </si>
+  <si>
+    <t>tc97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test GUI functionality </t>
   </si>
 </sst>
 </file>
@@ -596,7 +923,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -615,8 +942,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -652,11 +985,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -668,9 +1014,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -698,20 +1041,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -724,12 +1105,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -849,6 +1224,13 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -866,13 +1248,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1071,31 +1446,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E450872-46DF-4A3C-BD66-0891C0DB87E4}" name="Table1" displayName="Table1" ref="A3:H50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A3:H50" xr:uid="{2E450872-46DF-4A3C-BD66-0891C0DB87E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E450872-46DF-4A3C-BD66-0891C0DB87E4}" name="Table1" displayName="Table1" ref="A3:H100" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A3:H100" xr:uid="{2E450872-46DF-4A3C-BD66-0891C0DB87E4}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2A1C62DC-7615-47AA-BE31-3F6BBA36C62E}" name="TEST NO" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{986996CD-5EE4-4522-B08F-E76D83A83D4C}" name="TEST ID" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{FE730A53-5EEF-4A76-BCD9-2A805E39482D}" name="OBJECTIVE" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{4B96D5CC-2EAF-4A43-8704-8ABDE2CD6F46}" name="STEPS" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{94AF5410-28EC-43D6-BB8D-0CA5EEAE7B73}" name="INPUT" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{1EA1E4D4-1533-438A-BF78-61C21075C0C6}" name="EXEPECTED OUTPUT" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{F106BA7F-BA18-414A-82D0-4EF16551729D}" name="OUTPUT" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{BE678DB3-711B-4929-81C6-B84C97563F39}" name="COMMENTS/ERROR(S)" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{2A1C62DC-7615-47AA-BE31-3F6BBA36C62E}" name="TEST NO" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{986996CD-5EE4-4522-B08F-E76D83A83D4C}" name="TEST ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{FE730A53-5EEF-4A76-BCD9-2A805E39482D}" name="OBJECTIVE" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{4B96D5CC-2EAF-4A43-8704-8ABDE2CD6F46}" name="STEPS" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{94AF5410-28EC-43D6-BB8D-0CA5EEAE7B73}" name="INPUT" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{1EA1E4D4-1533-438A-BF78-61C21075C0C6}" name="EXEPECTED OUTPUT" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{F106BA7F-BA18-414A-82D0-4EF16551729D}" name="OUTPUT" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{BE678DB3-711B-4929-81C6-B84C97563F39}" name="COMMENTS/ERROR(S)" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51536A3D-D140-4760-98C2-8F29F192E818}" name="Table2" displayName="Table2" ref="A4:E25" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="6">
-  <autoFilter ref="A4:E25" xr:uid="{51536A3D-D140-4760-98C2-8F29F192E818}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0215BD31-DDF8-4299-B6FC-FFE5C32C38CD}" name="Error" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4C3E167D-F091-46DB-9E55-A98E586F6F59}" name="ERROR ID" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4330AAF2-23C8-4315-BE23-84C064621338}" name="ISSUE" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{A235DADF-B4F0-43EF-A6D6-64A4C188D5A7}" name="ERROR DESCRIPTION" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{6AE35E81-F80B-47F9-8503-50D2DD844005}" name="COMMENTS" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51536A3D-D140-4760-98C2-8F29F192E818}" name="Table2" displayName="Table2" ref="A4:F25" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A4:F25" xr:uid="{51536A3D-D140-4760-98C2-8F29F192E818}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{0215BD31-DDF8-4299-B6FC-FFE5C32C38CD}" name="Error" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4C3E167D-F091-46DB-9E55-A98E586F6F59}" name="ERROR ID" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{4330AAF2-23C8-4315-BE23-84C064621338}" name="ISSUE" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A235DADF-B4F0-43EF-A6D6-64A4C188D5A7}" name="ERROR DESCRIPTION" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{6AE35E81-F80B-47F9-8503-50D2DD844005}" name="COMMENTS" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{AB070037-101D-4A8E-8FE1-F527FA4E7CCF}" name="STATE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1369,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14B6601-0E27-48C2-8B67-D3F95DE45290}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1380,14 +1756,14 @@
     <col min="1" max="1" width="9.8984375" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="55.5" customWidth="1"/>
-    <col min="4" max="4" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="55.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="75.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
@@ -1431,16 +1807,16 @@
       <c r="D4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -1455,16 +1831,16 @@
       <c r="D5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -1479,16 +1855,16 @@
       <c r="D6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="11"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1503,16 +1879,16 @@
       <c r="D7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -1527,16 +1903,16 @@
       <c r="D8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -1551,16 +1927,16 @@
       <c r="D9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -1575,16 +1951,16 @@
       <c r="D10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1599,16 +1975,16 @@
       <c r="D11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -1623,16 +1999,16 @@
       <c r="D12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -1647,16 +2023,16 @@
       <c r="D13" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -1671,16 +2047,16 @@
       <c r="D14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1695,16 +2071,16 @@
       <c r="D15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -1719,16 +2095,16 @@
       <c r="D16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="11"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -1743,16 +2119,16 @@
       <c r="D17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -1770,13 +2146,13 @@
       <c r="E18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -1791,16 +2167,16 @@
       <c r="D19" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -1815,16 +2191,16 @@
       <c r="D20" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>15</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>15</v>
       </c>
-      <c r="H20" s="11"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -1839,16 +2215,16 @@
       <c r="D21" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>1000</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="7">
         <v>1000</v>
       </c>
-      <c r="H21" s="11"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1863,16 +2239,16 @@
       <c r="D22" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>-14</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>-14</v>
       </c>
-      <c r="H22" s="11"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -1887,16 +2263,16 @@
       <c r="D23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>0.02</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>0.02</v>
       </c>
-      <c r="H23" s="11"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
@@ -1911,16 +2287,16 @@
       <c r="D24" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>494.5</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="7">
         <v>494.5</v>
       </c>
-      <c r="H24" s="11"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -1938,13 +2314,13 @@
       <c r="E25" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>85</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="7">
         <v>85</v>
       </c>
-      <c r="H25" s="11"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
@@ -1962,13 +2338,13 @@
       <c r="E26" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>101</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="7">
         <v>101</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -1986,13 +2362,13 @@
       <c r="E27" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>118</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2012,13 +2388,13 @@
       <c r="E28" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>25</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="7">
         <v>25</v>
       </c>
-      <c r="H28" s="11"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
@@ -2036,13 +2412,13 @@
       <c r="E29" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>25</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="11" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2059,16 +2435,16 @@
       <c r="D30" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>1</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="7">
         <v>1</v>
       </c>
-      <c r="H30" s="11"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
@@ -2086,13 +2462,13 @@
       <c r="E31" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>-40</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="7">
         <v>-40</v>
       </c>
-      <c r="H31" s="11"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
@@ -2107,16 +2483,16 @@
       <c r="D32" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>-4</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="7">
         <v>-4</v>
       </c>
-      <c r="H32" s="11"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
@@ -2131,16 +2507,16 @@
       <c r="D33" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>44</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="7">
         <v>44</v>
       </c>
-      <c r="H33" s="11"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
@@ -2149,12 +2525,22 @@
       <c r="B34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="11"/>
+      <c r="C34" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" s="6">
+        <v>16</v>
+      </c>
+      <c r="G34" s="7">
+        <v>16</v>
+      </c>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
@@ -2163,12 +2549,22 @@
       <c r="B35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="11"/>
+      <c r="C35" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="6">
+        <v>83</v>
+      </c>
+      <c r="G35" s="7">
+        <v>83</v>
+      </c>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
@@ -2177,12 +2573,22 @@
       <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="11"/>
+      <c r="C36" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="6">
+        <v>29</v>
+      </c>
+      <c r="G36" s="7">
+        <v>29</v>
+      </c>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
@@ -2191,12 +2597,22 @@
       <c r="B37" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="11"/>
+      <c r="C37" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F37" s="6">
+        <v>4099</v>
+      </c>
+      <c r="G37" s="7">
+        <v>4099</v>
+      </c>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
@@ -2205,12 +2621,22 @@
       <c r="B38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="11"/>
+      <c r="C38" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F38" s="6">
+        <v>60</v>
+      </c>
+      <c r="G38" s="7">
+        <v>60</v>
+      </c>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
@@ -2219,12 +2645,22 @@
       <c r="B39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="11"/>
+      <c r="C39" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39" s="6">
+        <v>1619</v>
+      </c>
+      <c r="G39" s="7">
+        <v>1619</v>
+      </c>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
@@ -2233,12 +2669,24 @@
       <c r="B40" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="11"/>
+      <c r="C40" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="6">
+        <v>33</v>
+      </c>
+      <c r="G40" s="9">
+        <v>-27</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
@@ -2247,12 +2695,24 @@
       <c r="B41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="11"/>
+      <c r="C41" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" s="6">
+        <v>33</v>
+      </c>
+      <c r="G41" s="7">
+        <v>33</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
@@ -2261,12 +2721,22 @@
       <c r="B42" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="11"/>
+      <c r="C42" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" s="6">
+        <v>2</v>
+      </c>
+      <c r="G42" s="7">
+        <v>2</v>
+      </c>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
@@ -2275,12 +2745,22 @@
       <c r="B43" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="11"/>
+      <c r="C43" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F43" s="6">
+        <v>6</v>
+      </c>
+      <c r="G43" s="7">
+        <v>6</v>
+      </c>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
@@ -2289,12 +2769,22 @@
       <c r="B44" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="11"/>
+      <c r="C44" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F44" s="6">
+        <v>8</v>
+      </c>
+      <c r="G44" s="7">
+        <v>8</v>
+      </c>
+      <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
@@ -2303,12 +2793,22 @@
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="11"/>
+      <c r="C45" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F45" s="6">
+        <v>5</v>
+      </c>
+      <c r="G45" s="7">
+        <v>5</v>
+      </c>
+      <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
@@ -2317,12 +2817,22 @@
       <c r="B46" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="11"/>
+      <c r="C46" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F46" s="6">
+        <v>40</v>
+      </c>
+      <c r="G46" s="7">
+        <v>40</v>
+      </c>
+      <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
@@ -2331,12 +2841,22 @@
       <c r="B47" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="11"/>
+      <c r="C47" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F47" s="6">
+        <v>8</v>
+      </c>
+      <c r="G47" s="7">
+        <v>8</v>
+      </c>
+      <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
@@ -2345,12 +2865,22 @@
       <c r="B48" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="11"/>
+      <c r="C48" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="6">
+        <v>40</v>
+      </c>
+      <c r="G48" s="7">
+        <v>40</v>
+      </c>
+      <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
@@ -2359,12 +2889,22 @@
       <c r="B49" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="11"/>
+      <c r="C49" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F49" s="6">
+        <v>50</v>
+      </c>
+      <c r="G49" s="7">
+        <v>50</v>
+      </c>
+      <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
@@ -2373,15 +2913,804 @@
       <c r="B50" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="11"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C51" s="6"/>
+      <c r="C50" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F50" s="6">
+        <v>4</v>
+      </c>
+      <c r="G50" s="7">
+        <v>4</v>
+      </c>
+      <c r="H50" s="10"/>
+    </row>
+    <row r="51" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>48</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F51" s="6">
+        <v>200</v>
+      </c>
+      <c r="G51" s="7">
+        <v>200</v>
+      </c>
+      <c r="H51" s="14"/>
+    </row>
+    <row r="52" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>49</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F52" s="6">
+        <v>166.66</v>
+      </c>
+      <c r="G52" s="7">
+        <v>166.66</v>
+      </c>
+      <c r="H52" s="14"/>
+    </row>
+    <row r="53" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>50</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F53" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="G53" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="H53" s="14"/>
+    </row>
+    <row r="54" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>51</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F54" s="6">
+        <v>43</v>
+      </c>
+      <c r="G54" s="7">
+        <v>43</v>
+      </c>
+      <c r="H54" s="14"/>
+    </row>
+    <row r="55" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>52</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F55" s="6">
+        <v>94</v>
+      </c>
+      <c r="G55" s="7">
+        <v>94</v>
+      </c>
+      <c r="H55" s="14"/>
+    </row>
+    <row r="56" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>53</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F56" s="6">
+        <v>-3</v>
+      </c>
+      <c r="G56" s="7">
+        <v>-3</v>
+      </c>
+      <c r="H56" s="14"/>
+    </row>
+    <row r="57" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>54</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F57" s="6">
+        <v>1.73</v>
+      </c>
+      <c r="G57" s="7">
+        <v>1.73</v>
+      </c>
+      <c r="H57" s="14"/>
+    </row>
+    <row r="58" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>55</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D58" s="16"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>56</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D59" s="16"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>57</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D60" s="16"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>58</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D61" s="16"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>59</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>60</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D63" s="16"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="10"/>
+    </row>
+    <row r="64" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>61</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="10"/>
+    </row>
+    <row r="65" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>62</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>63</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="10"/>
+    </row>
+    <row r="67" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>64</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>65</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>66</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>67</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="10"/>
+    </row>
+    <row r="71" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>68</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>69</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>70</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>71</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>72</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="10"/>
+    </row>
+    <row r="76" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>73</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>74</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>75</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>76</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>77</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="10"/>
+    </row>
+    <row r="81" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>78</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="10"/>
+    </row>
+    <row r="82" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>79</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="10"/>
+    </row>
+    <row r="83" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>80</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C83" s="5"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="10"/>
+    </row>
+    <row r="84" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>81</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C84" s="5"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="10"/>
+    </row>
+    <row r="85" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>82</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="10"/>
+    </row>
+    <row r="86" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>83</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="10"/>
+    </row>
+    <row r="87" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>84</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="10"/>
+    </row>
+    <row r="88" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>85</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="10"/>
+    </row>
+    <row r="89" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>86</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="10"/>
+    </row>
+    <row r="90" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>87</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="10"/>
+    </row>
+    <row r="91" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>88</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="16"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="10"/>
+    </row>
+    <row r="92" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>89</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="10"/>
+    </row>
+    <row r="93" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>90</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
+      <c r="H93" s="10"/>
+    </row>
+    <row r="94" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>91</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="10"/>
+    </row>
+    <row r="95" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>92</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="16"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="19"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="10"/>
+    </row>
+    <row r="96" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>93</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="10"/>
+    </row>
+    <row r="97" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>94</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="16"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="10"/>
+    </row>
+    <row r="98" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>95</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="10"/>
+    </row>
+    <row r="99" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>96</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="16"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="19"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="10"/>
+    </row>
+    <row r="100" spans="1:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>97</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C100" s="20"/>
+      <c r="D100" s="21"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
+      <c r="H100" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2398,10 +3727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3F10F0-99DA-4AAD-92A9-79519DDF818A}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2410,15 +3739,16 @@
     <col min="2" max="2" width="15.09765625" customWidth="1"/>
     <col min="3" max="3" width="37.59765625" customWidth="1"/>
     <col min="4" max="4" width="89.19921875" customWidth="1"/>
-    <col min="5" max="5" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>129</v>
       </c>
@@ -2434,8 +3764,11 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -2445,156 +3778,187 @@
       <c r="C5" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="6"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="6"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="6"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="6"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="6"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="6"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="6"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="5"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="5"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="16"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>